<commit_message>
Upload LICENSE file, reintegrate CalculatePerformance and CalculateReverence helper functions tied into train() (WIP), and include Prediction vs. Error by Label visuals + FeatureWise summaries. Tag: v3.7.2
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">age</t>
   </si>
@@ -75,7 +75,7 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">Accuracy</t>
+    <t xml:space="preserve">Class</t>
   </si>
   <si>
     <t xml:space="preserve">Precision</t>
@@ -87,13 +87,10 @@
     <t xml:space="preserve">F1_Score</t>
   </si>
   <si>
-    <t xml:space="preserve">F1_Class0</t>
+    <t xml:space="preserve">Support</t>
   </si>
   <si>
-    <t xml:space="preserve">F1_Class1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macro_F1</t>
+    <t xml:space="preserve">Accuracy</t>
   </si>
   <si>
     <t xml:space="preserve">TP</t>
@@ -108,6 +105,12 @@
     <t xml:space="preserve">FN</t>
   </si>
   <si>
+    <t xml:space="preserve">macro avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weighted avg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Interpretation</t>
   </si>
   <si>
@@ -117,13 +120,22 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">Positive (1)</t>
+    <t xml:space="preserve">Actual</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative (0)</t>
+    <t xml:space="preserve">Predicted</t>
   </si>
   <si>
-    <t xml:space="preserve">Class</t>
+    <t xml:space="preserve">Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
   </si>
   <si>
     <t xml:space="preserve">MeanProbability</t>
@@ -132,13 +144,7 @@
     <t xml:space="preserve">StdDev</t>
   </si>
   <si>
-    <t xml:space="preserve">Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commentary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prediction means data is missing or does not include a 'prob' column.</t>
+    <t xml:space="preserve">✅ Since your model produces mean 0.0752 for true label 0, and 0.9075 for true label 1, it’s making sharp, confident, and accurate predictions.</t>
   </si>
   <si>
     <t xml:space="preserve">predicted_prob</t>
@@ -150,13 +156,16 @@
     <t xml:space="preserve">actual_label</t>
   </si>
   <si>
+    <t xml:space="preserve">error</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">False Positive</t>
+    <t xml:space="preserve">False Negative</t>
   </si>
   <si>
-    <t xml:space="preserve">False Negative</t>
+    <t xml:space="preserve">False Positive</t>
   </si>
 </sst>
 </file>
@@ -43086,86 +43095,213 @@
       <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.982625482625483</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.978846153846154</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.980732177263969</v>
+      </c>
+      <c r="E2" t="n">
+        <v>520</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="G2" t="n">
+        <v>271</v>
+      </c>
+      <c r="H2" t="n">
+        <v>509</v>
+      </c>
+      <c r="I2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.960992907801418</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.967857142857143</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.9644128113879</v>
+      </c>
+      <c r="E3" t="n">
+        <v>280</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="G3" t="n">
+        <v>271</v>
+      </c>
+      <c r="H3" t="n">
+        <v>509</v>
+      </c>
+      <c r="I3" t="n">
+        <v>11</v>
+      </c>
+      <c r="J3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+      <c r="B4" t="n">
+        <v>0.971809195213451</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.973351648351648</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.972572494325935</v>
+      </c>
+      <c r="E4" t="n">
+        <v>800</v>
+      </c>
+      <c r="F4" t="n">
         <v>0.975</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.960992907767341</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.967857142822577</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.964412806353643</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.980732177263969</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.9644128113879</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.972572494325935</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="G4" t="n">
         <v>271</v>
       </c>
-      <c r="I2" t="n">
+      <c r="H4" t="n">
         <v>509</v>
       </c>
-      <c r="J2" t="n">
+      <c r="I4" t="n">
         <v>11</v>
       </c>
-      <c r="K2" t="n">
+      <c r="J4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.97505408143706</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.975020399207345</v>
+      </c>
+      <c r="E5" t="n">
+        <v>800</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="G5" t="n">
+        <v>271</v>
+      </c>
+      <c r="H5" t="n">
+        <v>509</v>
+      </c>
+      <c r="I5" t="n">
+        <v>11</v>
+      </c>
+      <c r="J5" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="n">
-        <v>271</v>
-      </c>
-      <c r="C14" t="n">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="n">
+        <v>509</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="n">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="n">
         <v>9</v>
       </c>
-      <c r="C15" t="n">
-        <v>509</v>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="n">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -43185,16 +43321,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -43227,12 +43363,12 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -43251,13 +43387,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -43296,30 +43432,33 @@
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.998423891468001</v>
+        <v>0.00000653165408495955</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
       <c r="D2" t="n">
-        <v>0.0532232367871467</v>
+        <v>-0.000784742289868894</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.132347358479821</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.0463557834470937</v>
+        <v>-0.0551419790557054</v>
       </c>
       <c r="G2" t="n">
-        <v>0.140090033267649</v>
+        <v>-0.11259225485437</v>
       </c>
       <c r="H2" t="n">
         <v>-0.138460448550175</v>
@@ -43328,30 +43467,33 @@
         <v>-0.0955199418171921</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.00217767286457587</v>
+        <v>-0.0712112368452979</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.0203809007240386</v>
+        <v>0.0418374468810857</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.0231559509166694</v>
+        <v>-0.0516607420523233</v>
       </c>
       <c r="M2" t="n">
         <v>0.0937126778396502</v>
       </c>
       <c r="N2" t="n">
-        <v>0.188276232951694</v>
+        <v>-0.0837761223546214</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0372117479260586</v>
-      </c>
-      <c r="P2" t="s">
-        <v>45</v>
+        <v>-0.0801128775044263</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.999993468345915</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.9715689986555</v>
+        <v>0.998423891468001</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -43360,16 +43502,16 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.128834407494968</v>
+        <v>0.0532232367871467</v>
       </c>
       <c r="E3" t="n">
-        <v>0.132347358479821</v>
+        <v>-0.119179203192282</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0606647305811184</v>
+        <v>-0.0463557834470937</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.140090033267649</v>
       </c>
       <c r="H3" t="n">
         <v>-0.138460448550175</v>
@@ -43378,89 +43520,95 @@
         <v>-0.0955199418171921</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.0373220327093071</v>
+        <v>-0.00217767286457587</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0452682397660883</v>
+        <v>-0.0203809007240386</v>
       </c>
       <c r="L3" t="n">
-        <v>0.090863213625946</v>
+        <v>-0.0231559509166694</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.168312901646214</v>
+        <v>0.0937126778396502</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.188276232951694</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.107814525175513</v>
-      </c>
-      <c r="P3" t="s">
-        <v>45</v>
+        <v>0.0372117479260586</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.998423891468001</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.953029377141658</v>
+        <v>0.0121192758121339</v>
       </c>
       <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
       <c r="D4" t="n">
-        <v>-0.0223879339206751</v>
+        <v>0.193643982387387</v>
       </c>
       <c r="E4" t="n">
         <v>0.132347358479821</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.0577778377382889</v>
+        <v>-0.0664385162667775</v>
       </c>
       <c r="G4" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H4" t="n">
-        <v>0.245122216505601</v>
+        <v>0.0259321221880144</v>
       </c>
       <c r="I4" t="n">
-        <v>0.165128374537907</v>
+        <v>-0.0955199418171921</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.0599148354666343</v>
+        <v>0.0128841956403089</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0452682397660883</v>
+        <v>-0.0825992483291629</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1193680047616</v>
+        <v>0.00534884021898446</v>
       </c>
       <c r="M4" t="n">
         <v>0.0937126778396502</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.188276232951694</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.0784833688178918</v>
-      </c>
-      <c r="P4" t="s">
-        <v>45</v>
+        <v>0.0909855345816975</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.987880724187866</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.936012812594198</v>
+        <v>0.0259176597676445</v>
       </c>
       <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
       <c r="D5" t="n">
-        <v>0.161239194941178</v>
+        <v>-0.162808679520916</v>
       </c>
       <c r="E5" t="n">
         <v>-0.119179203192282</v>
@@ -43472,7 +43620,7 @@
         <v>0.140090033267649</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0836629249707786</v>
+        <v>0.00401311275625581</v>
       </c>
       <c r="I5" t="n">
         <v>0.165128374537907</v>
@@ -43481,10 +43629,10 @@
         <v>-0.00423860088365631</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0580142172584181</v>
+        <v>-0.0228696346282436</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.0801655331879771</v>
+        <v>0.00534884021898446</v>
       </c>
       <c r="M5" t="n">
         <v>-0.168312901646214</v>
@@ -43493,15 +43641,18 @@
         <v>-0.0837761223546214</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.176253890009963</v>
-      </c>
-      <c r="P5" t="s">
-        <v>45</v>
+        <v>0.0877265172086285</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.974082340232356</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.898757922658311</v>
+        <v>0.9715689986555</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -43510,31 +43661,31 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0748264284179529</v>
+        <v>0.128834407494968</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.132347358479821</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.047736471328447</v>
+        <v>-0.0606647305811184</v>
       </c>
       <c r="G6" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00401311275625581</v>
+        <v>-0.138460448550175</v>
       </c>
       <c r="I6" t="n">
         <v>-0.0955199418171921</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0649354583015959</v>
+        <v>-0.0373220327093071</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0203809007240386</v>
+        <v>-0.0452682397660883</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.108670324323631</v>
+        <v>0.090863213625946</v>
       </c>
       <c r="M6" t="n">
         <v>-0.168312901646214</v>
@@ -43543,15 +43694,18 @@
         <v>-0.0837761223546214</v>
       </c>
       <c r="O6" t="n">
-        <v>0.185497038400699</v>
-      </c>
-      <c r="P6" t="s">
-        <v>45</v>
+        <v>-0.107814525175513</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.9715689986555</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.822025844766444</v>
+        <v>0.953029377141658</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -43560,48 +43714,51 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0748264284179529</v>
+        <v>-0.0223879339206751</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.132347358479821</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.00142066876305128</v>
+        <v>-0.0577778377382889</v>
       </c>
       <c r="G7" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H7" t="n">
-        <v>0.135527169346807</v>
+        <v>0.245122216505601</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.165128374537907</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.00423860088365631</v>
+        <v>-0.0599148354666343</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0228696346282436</v>
+        <v>-0.0452682397660883</v>
       </c>
       <c r="L7" t="n">
-        <v>0.00534884021898446</v>
+        <v>0.1193680047616</v>
       </c>
       <c r="M7" t="n">
         <v>0.0937126778396502</v>
       </c>
       <c r="N7" t="n">
-        <v>0.188276232951694</v>
+        <v>-0.0837761223546214</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0898899296236334</v>
-      </c>
-      <c r="P7" t="s">
-        <v>45</v>
+        <v>-0.0784833688178918</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.953029377141658</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.769065417750433</v>
+        <v>0.936012812594198</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -43610,31 +43767,31 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.195213466967125</v>
+        <v>0.161239194941178</v>
       </c>
       <c r="E8" t="n">
-        <v>0.132347358479821</v>
+        <v>-0.119179203192282</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.0430923393638951</v>
+        <v>-0.00142066876305128</v>
       </c>
       <c r="G8" t="n">
         <v>0.140090033267649</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.248055495708968</v>
+        <v>-0.0836629249707786</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.165128374537907</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.0674457697190767</v>
+        <v>-0.00423860088365631</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.00793723120301372</v>
+        <v>0.0580142172584181</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0231559509166694</v>
+        <v>-0.0801655331879771</v>
       </c>
       <c r="M8" t="n">
         <v>-0.168312901646214</v>
@@ -43643,15 +43800,18 @@
         <v>-0.0837761223546214</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.107814525175513</v>
-      </c>
-      <c r="P8" t="s">
-        <v>45</v>
+        <v>-0.176253890009963</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.936012812594198</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.769065417750433</v>
+        <v>0.898757922658311</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -43660,98 +43820,104 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.206015062782528</v>
+        <v>0.0748264284179529</v>
       </c>
       <c r="E9" t="n">
         <v>-0.119179203192282</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0558950815364435</v>
+        <v>-0.047736471328447</v>
       </c>
       <c r="G9" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0259321221880144</v>
+        <v>0.00401311275625581</v>
       </c>
       <c r="I9" t="n">
         <v>-0.0955199418171921</v>
       </c>
       <c r="J9" t="n">
-        <v>0.134634299388128</v>
+        <v>-0.0649354583015959</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.070155578808138</v>
+        <v>-0.0203809007240386</v>
       </c>
       <c r="L9" t="n">
-        <v>0.090863213625946</v>
+        <v>-0.108670324323631</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0937126778396502</v>
+        <v>-0.168312901646214</v>
       </c>
       <c r="N9" t="n">
-        <v>0.188276232951694</v>
+        <v>-0.0837761223546214</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.102925999115909</v>
-      </c>
-      <c r="P9" t="s">
-        <v>45</v>
+        <v>0.185497038400699</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.898757922658311</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.769065417750433</v>
+        <v>0.16461049433762</v>
       </c>
       <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
         <v>1</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
       <c r="D10" t="n">
-        <v>-0.1088007004439</v>
+        <v>0.269255153095209</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.132347358479821</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.0345571779155295</v>
+        <v>0.0397489335173005</v>
       </c>
       <c r="G10" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0259321221880144</v>
+        <v>0.135527169346807</v>
       </c>
       <c r="I10" t="n">
-        <v>0.165128374537907</v>
+        <v>-0.0955199418171921</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0241805970189726</v>
+        <v>-0.0398323441267879</v>
       </c>
       <c r="K10" t="n">
-        <v>0.116499464007235</v>
+        <v>-0.00793723120301372</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.165679906594939</v>
+        <v>-0.0801655331879771</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.168312901646214</v>
+        <v>0.0937126778396502</v>
       </c>
       <c r="N10" t="n">
         <v>-0.0837761223546214</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.115962068608186</v>
-      </c>
-      <c r="P10" t="s">
-        <v>45</v>
+        <v>-0.0165620387295803</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.83538950566238</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.709433863252301</v>
+        <v>0.822025844766444</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -43760,25 +43926,25 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.226048769833596</v>
+        <v>0.0748264284179529</v>
       </c>
       <c r="E11" t="n">
         <v>-0.119179203192282</v>
       </c>
       <c r="F11" t="n">
-        <v>0.495375934363876</v>
+        <v>-0.00142066876305128</v>
       </c>
       <c r="G11" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.0288654013913821</v>
+        <v>0.135527169346807</v>
       </c>
       <c r="I11" t="n">
         <v>-0.0955199418171921</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.0448529669617495</v>
+        <v>-0.00423860088365631</v>
       </c>
       <c r="K11" t="n">
         <v>-0.0228696346282436</v>
@@ -43793,15 +43959,18 @@
         <v>0.188276232951694</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.0393751603410635</v>
-      </c>
-      <c r="P11" t="s">
-        <v>45</v>
+        <v>-0.0898899296236334</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.822025844766444</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.645049692487488</v>
+        <v>0.769065417750433</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -43810,31 +43979,31 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0100168535255342</v>
+        <v>-0.195213466967125</v>
       </c>
       <c r="E12" t="n">
         <v>0.132347358479821</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.0639281746643171</v>
+        <v>-0.0430923393638951</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.140090033267649</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0259321221880144</v>
+        <v>-0.248055495708968</v>
       </c>
       <c r="I12" t="n">
-        <v>0.165128374537907</v>
+        <v>-0.0955199418171921</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.0473632783792303</v>
+        <v>-0.0674457697190767</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0577119092871132</v>
+        <v>-0.00793723120301372</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1193680047616</v>
+        <v>-0.0231559509166694</v>
       </c>
       <c r="M12" t="n">
         <v>-0.168312901646214</v>
@@ -43843,98 +44012,104 @@
         <v>-0.0837761223546214</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.03448663428146</v>
-      </c>
-      <c r="P12" t="s">
-        <v>45</v>
+        <v>-0.107814525175513</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.769065417750433</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.593423476405454</v>
+        <v>0.769065417750433</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.162808679520916</v>
+        <v>-0.206015062782528</v>
       </c>
       <c r="E13" t="n">
         <v>-0.119179203192282</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.0358123487167598</v>
+        <v>-0.0558950815364435</v>
       </c>
       <c r="G13" t="n">
-        <v>0.140090033267649</v>
+        <v>-0.11259225485437</v>
       </c>
       <c r="H13" t="n">
-        <v>0.245122216505601</v>
+        <v>0.0259321221880144</v>
       </c>
       <c r="I13" t="n">
-        <v>0.165128374537907</v>
+        <v>-0.0955199418171921</v>
       </c>
       <c r="J13" t="n">
-        <v>0.138399766514349</v>
+        <v>0.134634299388128</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.0452682397660883</v>
+        <v>-0.070155578808138</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.0231559509166694</v>
+        <v>0.090863213625946</v>
       </c>
       <c r="M13" t="n">
         <v>0.0937126778396502</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.188276232951694</v>
       </c>
       <c r="O13" t="n">
-        <v>0.089356025895163</v>
-      </c>
-      <c r="P13" t="s">
-        <v>46</v>
+        <v>-0.102925999115909</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.769065417750433</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.593423476405454</v>
+        <v>0.769065417750433</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0547927213668844</v>
+        <v>-0.1088007004439</v>
       </c>
       <c r="E14" t="n">
         <v>-0.119179203192282</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0685723066288689</v>
+        <v>-0.0345571779155295</v>
       </c>
       <c r="G14" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0807296457674109</v>
+        <v>0.0259321221880144</v>
       </c>
       <c r="I14" t="n">
         <v>0.165128374537907</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0718765139511078</v>
+        <v>0.0241805970189726</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.0577119092871132</v>
+        <v>0.116499464007235</v>
       </c>
       <c r="L14" t="n">
-        <v>0.090863213625946</v>
+        <v>-0.165679906594939</v>
       </c>
       <c r="M14" t="n">
         <v>-0.168312901646214</v>
@@ -43943,45 +44118,48 @@
         <v>-0.0837761223546214</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.0931489469967024</v>
-      </c>
-      <c r="P14" t="s">
-        <v>46</v>
+        <v>-0.115962068608186</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.769065417750433</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.550271330029102</v>
+        <v>0.709433863252301</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.0763959129976906</v>
+        <v>0.226048769833596</v>
       </c>
       <c r="E15" t="n">
-        <v>0.132347358479821</v>
+        <v>-0.119179203192282</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0142689662523267</v>
+        <v>0.495375934363876</v>
       </c>
       <c r="G15" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00401311275625581</v>
+        <v>-0.0288654013913821</v>
       </c>
       <c r="I15" t="n">
         <v>-0.0955199418171921</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0794074482035502</v>
+        <v>-0.0448529669617495</v>
       </c>
       <c r="K15" t="n">
-        <v>0.00450643831801113</v>
+        <v>-0.0228696346282436</v>
       </c>
       <c r="L15" t="n">
         <v>0.00534884021898446</v>
@@ -43993,15 +44171,18 @@
         <v>0.188276232951694</v>
       </c>
       <c r="O15" t="n">
-        <v>0.126834725685457</v>
-      </c>
-      <c r="P15" t="s">
-        <v>46</v>
+        <v>-0.0393751603410635</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.709433863252301</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.500296435167104</v>
+        <v>0.333763778013851</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -44010,98 +44191,104 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.195213466967125</v>
+        <v>-0.000784742289868894</v>
       </c>
       <c r="E16" t="n">
         <v>-0.119179203192282</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0664385162667775</v>
+        <v>-0.0659364479462854</v>
       </c>
       <c r="G16" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0259321221880144</v>
+        <v>-0.193257972129572</v>
       </c>
       <c r="I16" t="n">
         <v>-0.0955199418171921</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.0975695067288463</v>
+        <v>-0.185430406340674</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.0825992483291629</v>
+        <v>0.191161481133384</v>
       </c>
       <c r="L16" t="n">
-        <v>0.090863213625946</v>
+        <v>-0.279699071137554</v>
       </c>
       <c r="M16" t="n">
         <v>0.0937126778396502</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.188276232951694</v>
       </c>
       <c r="O16" t="n">
-        <v>0.185497038400699</v>
-      </c>
-      <c r="P16" t="s">
-        <v>46</v>
+        <v>-0.109444033862048</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.666236221986149</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.333763778013851</v>
+        <v>0.645049692487488</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.000784742289868894</v>
+        <v>0.0100168535255342</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.132347358479821</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.0659364479462854</v>
+        <v>-0.0639281746643171</v>
       </c>
       <c r="G17" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.193257972129572</v>
+        <v>0.0259321221880144</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.165128374537907</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.185430406340674</v>
+        <v>-0.0473632783792303</v>
       </c>
       <c r="K17" t="n">
-        <v>0.191161481133384</v>
+        <v>-0.0577119092871132</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.279699071137554</v>
+        <v>0.1193680047616</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0937126778396502</v>
+        <v>-0.168312901646214</v>
       </c>
       <c r="N17" t="n">
-        <v>0.188276232951694</v>
+        <v>-0.0837761223546214</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.109444033862048</v>
-      </c>
-      <c r="P17" t="s">
-        <v>46</v>
+        <v>-0.03448663428146</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.645049692487488</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.16461049433762</v>
+        <v>0.500296435167104</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -44110,31 +44297,31 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0.269255153095209</v>
+        <v>-0.195213466967125</v>
       </c>
       <c r="E18" t="n">
-        <v>0.132347358479821</v>
+        <v>-0.119179203192282</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0397489335173005</v>
+        <v>-0.0664385162667775</v>
       </c>
       <c r="G18" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H18" t="n">
-        <v>0.135527169346807</v>
+        <v>0.0259321221880144</v>
       </c>
       <c r="I18" t="n">
         <v>-0.0955199418171921</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.0398323441267879</v>
+        <v>-0.0975695067288463</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.00793723120301372</v>
+        <v>-0.0825992483291629</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.0801655331879771</v>
+        <v>0.090863213625946</v>
       </c>
       <c r="M18" t="n">
         <v>0.0937126778396502</v>
@@ -44143,15 +44330,18 @@
         <v>-0.0837761223546214</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.0165620387295803</v>
-      </c>
-      <c r="P18" t="s">
-        <v>46</v>
+        <v>0.185497038400699</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.499703564832896</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.0259176597676445</v>
+        <v>0.550271330029102</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -44160,48 +44350,51 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.162808679520916</v>
+        <v>-0.0763959129976906</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.132347358479821</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.00142066876305128</v>
+        <v>0.0142689662523267</v>
       </c>
       <c r="G19" t="n">
-        <v>0.140090033267649</v>
+        <v>-0.11259225485437</v>
       </c>
       <c r="H19" t="n">
         <v>0.00401311275625581</v>
       </c>
       <c r="I19" t="n">
-        <v>0.165128374537907</v>
+        <v>-0.0955199418171921</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.00423860088365631</v>
+        <v>0.0794074482035502</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.0228696346282436</v>
+        <v>0.00450643831801113</v>
       </c>
       <c r="L19" t="n">
         <v>0.00534884021898446</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.168312901646214</v>
+        <v>0.0937126778396502</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.188276232951694</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0877265172086285</v>
-      </c>
-      <c r="P19" t="s">
-        <v>46</v>
+        <v>0.126834725685457</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.449728669970898</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.0121192758121339</v>
+        <v>0.593423476405454</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -44210,48 +44403,51 @@
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0.193643982387387</v>
+        <v>-0.162808679520916</v>
       </c>
       <c r="E20" t="n">
-        <v>0.132347358479821</v>
+        <v>-0.119179203192282</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.0664385162667775</v>
+        <v>-0.0358123487167598</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.140090033267649</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0259321221880144</v>
+        <v>0.245122216505601</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.165128374537907</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0128841956403089</v>
+        <v>0.138399766514349</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0825992483291629</v>
+        <v>-0.0452682397660883</v>
       </c>
       <c r="L20" t="n">
-        <v>0.00534884021898446</v>
+        <v>-0.0231559509166694</v>
       </c>
       <c r="M20" t="n">
         <v>0.0937126778396502</v>
       </c>
       <c r="N20" t="n">
-        <v>0.188276232951694</v>
+        <v>-0.0837761223546214</v>
       </c>
       <c r="O20" t="n">
-        <v>0.0909855345816975</v>
-      </c>
-      <c r="P20" t="s">
-        <v>46</v>
+        <v>0.089356025895163</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.406576523594546</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.00000653165408495955</v>
+        <v>0.593423476405454</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -44260,43 +44456,46 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.000784742289868894</v>
+        <v>-0.0547927213668844</v>
       </c>
       <c r="E21" t="n">
-        <v>0.132347358479821</v>
+        <v>-0.119179203192282</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.0551419790557054</v>
+        <v>-0.0685723066288689</v>
       </c>
       <c r="G21" t="n">
         <v>-0.11259225485437</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.138460448550175</v>
+        <v>0.0807296457674109</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.165128374537907</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.0712112368452979</v>
+        <v>0.0718765139511078</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0418374468810857</v>
+        <v>-0.0577119092871132</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.0516607420523233</v>
+        <v>0.090863213625946</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0937126778396502</v>
+        <v>-0.168312901646214</v>
       </c>
       <c r="N21" t="n">
         <v>-0.0837761223546214</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.0801128775044263</v>
-      </c>
-      <c r="P21" t="s">
-        <v>46</v>
+        <v>-0.0931489469967024</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.406576523594546</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -44315,7 +44514,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -44332,7 +44531,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" t="n">
         <v>-0.0211877566078525</v>
@@ -44349,7 +44548,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B3" t="n">
         <v>0.0178725595731001</v>

</xml_diff>

<commit_message>
Version 3.8 — Added evaluate_predictions_report.R and utils.R. Fixed performance and relevance helper functions including calculatePerformance() and calculateRelevance(). Passed best weights and biases from train_with_l2_regularization instead of relying on global variables. Helper functions now accept best_weights_record and best_biases_record directly, along with predicted_output, error, and dim_hidden_layers. Added verbose support to all evaluation metrics. utils.R created to store shared functions such as threshold_function and tune_threshold_accuracy(). Updated store_metadata() and prestore_metadata() to save best_weights_record, best_biases_record, and dim_hidden_layers. Restored ensemble evaluation logic. Ensemble pruning and addition will be reintroduced in a future version.
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">age</t>
   </si>
@@ -114,7 +114,13 @@
     <t xml:space="preserve">Interpretation</t>
   </si>
   <si>
-    <t xml:space="preserve">Excellent performance: model is highly accurate and balanced.</t>
+    <t xml:space="preserve">Accuracy: 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1 Score: 0.9644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">✅ Balanced precision and recall.</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -43234,18 +43240,23 @@
         <v>32</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
@@ -43264,7 +43275,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -43278,7 +43289,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -43292,7 +43303,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -43324,13 +43335,13 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -43368,7 +43379,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -43387,13 +43398,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -43432,10 +43443,10 @@
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
@@ -43449,46 +43460,46 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.000784742289868894</v>
+        <v>8.16460371854308</v>
       </c>
       <c r="E2" t="n">
-        <v>0.132347358479821</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.0551419790557054</v>
+        <v>14.8218959813551</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.138460448550175</v>
+        <v>4.3963250792155</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.0712112368452979</v>
+        <v>45847.3901118188</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0418374468810857</v>
+        <v>0.138170216775344</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.0516607420523233</v>
+        <v>17.4596910288844</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.0801128775044263</v>
+        <v>25.1218575955172</v>
       </c>
       <c r="P2" t="n">
         <v>0.999993468345915</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -43502,46 +43513,46 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0532232367871467</v>
+        <v>10.6767894780948</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0463557834470937</v>
+        <v>134.527547423994</v>
       </c>
       <c r="G3" t="n">
-        <v>0.140090033267649</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.138460448550175</v>
+        <v>7.53655727865515</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.00217767286457587</v>
+        <v>63683.909004636</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0203809007240386</v>
+        <v>0.401949721528275</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.0231559509166694</v>
+        <v>17.3340817409068</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0937126778396502</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.188276232951694</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0372117479260586</v>
+        <v>11.8072730698931</v>
       </c>
       <c r="P3" t="n">
         <v>0.998423891468001</v>
       </c>
       <c r="Q3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -43555,46 +43566,46 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.193643982387387</v>
+        <v>6.53168297483446</v>
       </c>
       <c r="E4" t="n">
-        <v>0.132347358479821</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.0664385162667775</v>
+        <v>23.8657647157413</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0259321221880144</v>
+        <v>4.77315294314826</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0128841956403089</v>
+        <v>47982.7480074378</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0825992483291629</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="L4" t="n">
-        <v>0.00534884021898446</v>
+        <v>17.585300316862</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N4" t="n">
-        <v>0.188276232951694</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0909855345816975</v>
+        <v>32.4071962982171</v>
       </c>
       <c r="P4" t="n">
         <v>0.987880724187866</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -43608,46 +43619,46 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.162808679520916</v>
+        <v>8.79265015843101</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.00142066876305128</v>
+        <v>73.1046056029549</v>
       </c>
       <c r="G5" t="n">
-        <v>0.140090033267649</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H5" t="n">
-        <v>0.00401311275625581</v>
+        <v>4.77315294314826</v>
       </c>
       <c r="I5" t="n">
-        <v>0.165128374537907</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.00423860088365631</v>
+        <v>3152.7931282374</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0228696346282436</v>
+        <v>0.138170216775344</v>
       </c>
       <c r="L5" t="n">
-        <v>0.00534884021898446</v>
+        <v>17.585300316862</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.168312901646214</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0877265172086285</v>
+        <v>30.8998848424861</v>
       </c>
       <c r="P5" t="n">
         <v>0.974082340232356</v>
       </c>
       <c r="Q5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -43661,46 +43672,46 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.128834407494968</v>
+        <v>8.79265015843101</v>
       </c>
       <c r="E6" t="n">
-        <v>0.132347358479821</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0606647305811184</v>
+        <v>65.4424390363222</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.138460448550175</v>
+        <v>5.65241795899136</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0373220327093071</v>
+        <v>23237.7182758534</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0452682397660883</v>
+        <v>0.150731145573103</v>
       </c>
       <c r="L6" t="n">
-        <v>0.090863213625946</v>
+        <v>17.4596910288844</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.168312901646214</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.107814525175513</v>
+        <v>4.14510650326033</v>
       </c>
       <c r="P6" t="n">
         <v>0.9715689986555</v>
       </c>
       <c r="Q6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7">
@@ -43714,46 +43725,46 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0223879339206751</v>
+        <v>8.03899443056549</v>
       </c>
       <c r="E7" t="n">
-        <v>0.132347358479821</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.0577778377382889</v>
+        <v>202.230953643913</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.245122216505601</v>
+        <v>3.14023219943964</v>
       </c>
       <c r="I7" t="n">
-        <v>0.165128374537907</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0599148354666343</v>
+        <v>38310.8328331637</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0452682397660883</v>
+        <v>0.26377950475293</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1193680047616</v>
+        <v>16.3292074370862</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0784833688178918</v>
+        <v>13.5658031015793</v>
       </c>
       <c r="P7" t="n">
         <v>0.953029377141658</v>
       </c>
       <c r="Q7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8">
@@ -43767,46 +43778,46 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.161239194941178</v>
+        <v>8.16460371854308</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.119179203192282</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.00142066876305128</v>
+        <v>73.1046056029549</v>
       </c>
       <c r="G8" t="n">
-        <v>0.140090033267649</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.0836629249707786</v>
+        <v>5.02437151910343</v>
       </c>
       <c r="I8" t="n">
-        <v>0.165128374537907</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.00423860088365631</v>
+        <v>3391.45077539482</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0580142172584181</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0801655331879771</v>
+        <v>17.3340817409068</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.168312901646214</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.176253890009963</v>
+        <v>17.585300316862</v>
       </c>
       <c r="P8" t="n">
         <v>0.936012812594198</v>
       </c>
       <c r="Q8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
@@ -43820,46 +43831,46 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0748264284179529</v>
+        <v>10.6767894780948</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.047736471328447</v>
+        <v>36.5523028014775</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00401311275625581</v>
+        <v>7.53655727865515</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0649354583015959</v>
+        <v>63683.909004636</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0203809007240386</v>
+        <v>0.401949721528275</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.108670324323631</v>
+        <v>17.3340817409068</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.168312901646214</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>0.185497038400699</v>
+        <v>11.8072730698931</v>
       </c>
       <c r="P9" t="n">
         <v>0.898757922658311</v>
       </c>
       <c r="Q9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -43873,46 +43884,46 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.269255153095209</v>
+        <v>7.28533870269997</v>
       </c>
       <c r="E10" t="n">
-        <v>0.132347358479821</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0397489335173005</v>
+        <v>18.0877374687724</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H10" t="n">
-        <v>0.135527169346807</v>
+        <v>4.77315294314826</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.0398323441267879</v>
+        <v>18464.5653327051</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.00793723120301372</v>
+        <v>0.08792650158431</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.0801655331879771</v>
+        <v>17.8365188928172</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.0165620387295803</v>
+        <v>10.4255709021396</v>
       </c>
       <c r="P10" t="n">
         <v>0.83538950566238</v>
       </c>
       <c r="Q10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11">
@@ -43926,46 +43937,46 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0748264284179529</v>
+        <v>5.90363653494653</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.00142066876305128</v>
+        <v>73.1046056029549</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.135527169346807</v>
+        <v>3.14023219943964</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.00423860088365631</v>
+        <v>16329.2074370862</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0228696346282436</v>
+        <v>0.100487430382069</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00534884021898446</v>
+        <v>16.8316445889965</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N11" t="n">
-        <v>0.188276232951694</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.0898899296236334</v>
+        <v>25.2474668834947</v>
       </c>
       <c r="P11" t="n">
         <v>0.822025844766444</v>
       </c>
       <c r="Q11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
@@ -43979,46 +43990,46 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.195213466967125</v>
+        <v>11.9328823578706</v>
       </c>
       <c r="E12" t="n">
-        <v>0.132347358479821</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.0430923393638951</v>
+        <v>14.0682402534896</v>
       </c>
       <c r="G12" t="n">
-        <v>0.140090033267649</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.248055495708968</v>
+        <v>5.02437151910343</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.0674457697190767</v>
+        <v>24619.4204436068</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.00793723120301372</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.0231559509166694</v>
+        <v>17.3340817409068</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.168312901646214</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.107814525175513</v>
+        <v>3.01462291146206</v>
       </c>
       <c r="P12" t="n">
         <v>0.769065417750433</v>
       </c>
       <c r="Q12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
@@ -44032,46 +44043,46 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.206015062782528</v>
+        <v>6.28046439887929</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.0558950815364435</v>
+        <v>73.1046056029549</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0259321221880144</v>
+        <v>3.76827863932757</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0.134634299388128</v>
+        <v>29141.3548107999</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.070155578808138</v>
+        <v>0.08792650158431</v>
       </c>
       <c r="L13" t="n">
-        <v>0.090863213625946</v>
+        <v>17.0828631649517</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0937126778396502</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0.188276232951694</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.102925999115909</v>
+        <v>30.8998848424861</v>
       </c>
       <c r="P13" t="n">
         <v>0.769065417750433</v>
       </c>
       <c r="Q13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
@@ -44085,46 +44096,46 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.1088007004439</v>
+        <v>7.28533870269997</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0345571779155295</v>
+        <v>16.7060353010189</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0259321221880144</v>
+        <v>7.53655727865515</v>
       </c>
       <c r="I14" t="n">
-        <v>0.165128374537907</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0241805970189726</v>
+        <v>33537.6798900154</v>
       </c>
       <c r="K14" t="n">
-        <v>0.116499464007235</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.165679906594939</v>
+        <v>17.7109096048396</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.168312901646214</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.115962068608186</v>
+        <v>10.4255709021396</v>
       </c>
       <c r="P14" t="n">
         <v>0.769065417750433</v>
       </c>
       <c r="Q14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -44138,46 +44149,46 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.226048769833596</v>
+        <v>5.2755900950586</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.119179203192282</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.495375934363876</v>
+        <v>12.8121473737137</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.0288654013913821</v>
+        <v>3.14023219943964</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.0448529669617495</v>
+        <v>29769.4012506878</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.0228696346282436</v>
+        <v>0.150731145573103</v>
       </c>
       <c r="L15" t="n">
-        <v>0.00534884021898446</v>
+        <v>16.8316445889965</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0937126778396502</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>0.188276232951694</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.0393751603410635</v>
+        <v>9.29508731034135</v>
       </c>
       <c r="P15" t="n">
         <v>0.709433863252301</v>
       </c>
       <c r="Q15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
@@ -44191,46 +44202,46 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.000784742289868894</v>
+        <v>5.2755900950586</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.119179203192282</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0659364479462854</v>
+        <v>654.298781075244</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.193257972129572</v>
+        <v>6.28046439887929</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.185430406340674</v>
+        <v>38687.6606970964</v>
       </c>
       <c r="K16" t="n">
-        <v>0.191161481133384</v>
+        <v>0.163292074370862</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.279699071137554</v>
+        <v>17.2084724529293</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N16" t="n">
-        <v>0.188276232951694</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.109444033862048</v>
+        <v>10.92800805405</v>
       </c>
       <c r="P16" t="n">
         <v>0.666236221986149</v>
       </c>
       <c r="Q16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
@@ -44244,46 +44255,46 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0100168535255342</v>
+        <v>5.65241795899136</v>
       </c>
       <c r="E17" t="n">
-        <v>0.132347358479821</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.0639281746643171</v>
+        <v>73.1046056029549</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0259321221880144</v>
+        <v>3.76827863932757</v>
       </c>
       <c r="I17" t="n">
-        <v>0.165128374537907</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.0473632783792303</v>
+        <v>17082.8631649517</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.0577119092871132</v>
+        <v>0.138170216775344</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1193680047616</v>
+        <v>17.2084724529293</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.168312901646214</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.03448663428146</v>
+        <v>1.38170216775344</v>
       </c>
       <c r="P17" t="n">
         <v>0.645049692487488</v>
       </c>
       <c r="Q17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18">
@@ -44297,46 +44308,46 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.195213466967125</v>
+        <v>9.42069659831893</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.119179203192282</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.0664385162667775</v>
+        <v>73.1046056029549</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0259321221880144</v>
+        <v>3.14023219943964</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.0975695067288463</v>
+        <v>45470.5622478861</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.0825992483291629</v>
+        <v>0.213535789561896</v>
       </c>
       <c r="L18" t="n">
-        <v>0.090863213625946</v>
+        <v>17.4596910288844</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="O18" t="n">
-        <v>0.185497038400699</v>
+        <v>10.92800805405</v>
       </c>
       <c r="P18" t="n">
         <v>0.499703564832896</v>
       </c>
       <c r="Q18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
@@ -44350,46 +44361,46 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.0763959129976906</v>
+        <v>6.65729226281205</v>
       </c>
       <c r="E19" t="n">
-        <v>0.132347358479821</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0142689662523267</v>
+        <v>26.1267318993378</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.11259225485437</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0.00401311275625581</v>
+        <v>7.53655727865515</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.0955199418171921</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0794074482035502</v>
+        <v>31276.7127064189</v>
       </c>
       <c r="K19" t="n">
-        <v>0.00450643831801113</v>
+        <v>0.08792650158431</v>
       </c>
       <c r="L19" t="n">
-        <v>0.00534884021898446</v>
+        <v>17.3340817409068</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N19" t="n">
-        <v>0.188276232951694</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="O19" t="n">
-        <v>0.126834725685457</v>
+        <v>13.3145845256241</v>
       </c>
       <c r="P19" t="n">
         <v>0.449728669970898</v>
       </c>
       <c r="Q19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
@@ -44403,46 +44414,46 @@
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.162808679520916</v>
+        <v>6.65729226281205</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.0358123487167598</v>
+        <v>56.0217424380033</v>
       </c>
       <c r="G20" t="n">
-        <v>0.140090033267649</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0.245122216505601</v>
+        <v>5.65241795899136</v>
       </c>
       <c r="I20" t="n">
-        <v>0.165128374537907</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J20" t="n">
-        <v>0.138399766514349</v>
+        <v>34416.9449058585</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0452682397660883</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.0231559509166694</v>
+        <v>16.7060353010189</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0937126778396502</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>0.089356025895163</v>
+        <v>27.0059969151809</v>
       </c>
       <c r="P20" t="n">
         <v>0.406576523594546</v>
       </c>
       <c r="Q20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21">
@@ -44456,46 +44467,46 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.0547927213668844</v>
+        <v>7.6203386737362</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.119179203192282</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.0685723066288689</v>
+        <v>18.9670024846155</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.11259225485437</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0807296457674109</v>
+        <v>5.02437151910343</v>
       </c>
       <c r="I21" t="n">
-        <v>0.165128374537907</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0718765139511078</v>
+        <v>25121.8575955172</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0577119092871132</v>
+        <v>0.125609287977586</v>
       </c>
       <c r="L21" t="n">
-        <v>0.090863213625946</v>
+        <v>17.0828631649517</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.168312901646214</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.0837761223546214</v>
+        <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.0931489469967024</v>
+        <v>21.6047975321448</v>
       </c>
       <c r="P21" t="n">
         <v>0.406576523594546</v>
       </c>
       <c r="Q21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -44514,7 +44525,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -44531,36 +44542,36 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.0211877566078525</v>
+        <v>7.37838727191626</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.00683112724558929</v>
+        <v>0.133983240509425</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0210612312031792</v>
+        <v>5.14998080708102</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0312368827420987</v>
+        <v>20.2928783021566</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0178725595731001</v>
+        <v>8.06183248292505</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0125753262063048</v>
+        <v>0.188413931966379</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0159132594544338</v>
+        <v>5.02437151910343</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.0572997558929431</v>
+        <v>12.6522810071968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v5.3.1: Created EnsemblesRun and SingleRuns folders in Artifacts. Removed K var and now using num_networks in TestDesonn.R. Rewrote Clean50SeedsRunResults.R to read from these folders (fused for ensemble).
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.996</v>
+        <v>0.998666666666667</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.987179487179487</v>
+        <v>0.995689655172414</v>
       </c>
     </row>
     <row r="4">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.993548387096774</v>
+        <v>0.997840172786177</v>
       </c>
     </row>
     <row r="6">
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5</v>
+        <v>0.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OUTSTANDING RESULTS: DESONN > Keras at 360 epochs; 200-epoch results less relevant - Training: DESONN clearly surpasses Keras at 360 epochs. 200-epoch results are less relevant, since DESONN emphasizes generalization over longer runs and delivers stronger true test accuracy when fully trained. - Note: Keras may appear sharper at lower epochs but lacks the generality DESONN shows as training continues. - Init: using zero-initialized biases for these runs (biases[[layer]] <- matrix(0, nrow = hidden_sizes[layer], ncol = 1)); not using rnorm for biases here—will revisit later. - Cleanup: continued refactor of Clean50SeedsRunResults.R (still WIP). - Pipeline: section C needs to read from EnsemblesRuns test outputs for multi-seed runs.
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.996</v>
+        <v>0.99733333</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.98717949</v>
+        <v>0.995671</v>
       </c>
     </row>
     <row r="8">
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0.995671</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.99354839</v>
+        <v>0.995671</v>
       </c>
     </row>
     <row r="10">
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.998666666666667</v>
+        <v>0.997333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.995689655172414</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -793,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.991341991341991</v>
       </c>
     </row>
     <row r="5">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.997840172786177</v>
+        <v>0.995652173913043</v>
       </c>
     </row>
     <row r="6">
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.62</v>
+        <v>0.93</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +834,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0.999532901267005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v5.4.1 true 31-seed comparison (512–542), unified columns across single-run & ensemble, light cleanup in multiple files
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.99733333</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.995671</v>
+        <v>0.97468354</v>
       </c>
     </row>
     <row r="8">
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.995671</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.995671</v>
+        <v>0.98717949</v>
       </c>
     </row>
     <row r="10">
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.997333333333333</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.974683544303797</v>
       </c>
     </row>
     <row r="4">
@@ -793,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.991341991341991</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.995652173913043</v>
+        <v>0.987179487179487</v>
       </c>
     </row>
     <row r="6">
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +834,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.999532901267005</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v5.5.0 ensured epoch loss plot saves and fuse folder populates for scenario D; renamed all references from DESONN to DDESONN
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.99866667</v>
+        <v>0.99733333</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.99568966</v>
+        <v>0.995671</v>
       </c>
     </row>
     <row r="8">
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0.995671</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.99784017</v>
+        <v>0.995671</v>
       </c>
     </row>
     <row r="10">
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5</v>
+        <v>0.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v5.5.1 integrated activation_functions_predict and removed activation_functions_learn; activation_functions is now activation_functions_learn
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>518</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.99733333</v>
+        <v>0.45733333</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.995671</v>
+        <v>0.35987261</v>
       </c>
     </row>
     <row r="8">
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.995671</v>
+        <v>0.97835498</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.995671</v>
+        <v>0.52619325</v>
       </c>
     </row>
     <row r="10">
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.998666666666667</v>
+        <v>0.308</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.995689655172414</v>
+        <v>0.308</v>
       </c>
     </row>
     <row r="4">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.997840172786177</v>
+        <v>0.470948012232416</v>
       </c>
     </row>
     <row r="6">
@@ -834,7 +834,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.999991658951197</v>
+        <v>0.824787928834172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up learning time. added update_weights_block.R and update_biases_block.R move some helper fns from train_with_l2_regulization to utils.R ensured dropout mask gurad for SL in learn function.
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>402</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>117</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.45733333</v>
+        <v>0.664</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.35987261</v>
+        <v>0.4767184</v>
       </c>
     </row>
     <row r="8">
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.97835498</v>
+        <v>0.93073593</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.52619325</v>
+        <v>0.63049853</v>
       </c>
     </row>
     <row r="10">
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.308</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.308</v>
+        <v>0.766666666666667</v>
       </c>
     </row>
     <row r="4">
@@ -793,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.597402597402597</v>
       </c>
     </row>
     <row r="5">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.470948012232416</v>
+        <v>0.671532846715329</v>
       </c>
     </row>
     <row r="6">
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.09</v>
+        <v>0.78</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +834,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.824787928834172</v>
+        <v>0.875409754022471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.5.3: renamed all references from desonn to DDESONN for consistency
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>215</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>283</v>
+        <v>519</v>
       </c>
     </row>
     <row r="5">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.664</v>
+        <v>0.99866667</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4767184</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.93073593</v>
+        <v>0.995671</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.63049853</v>
+        <v>0.9978308</v>
       </c>
     </row>
     <row r="10">
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.82</v>
+        <v>0.997333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.766666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -793,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.597402597402597</v>
+        <v>0.991341991341991</v>
       </c>
     </row>
     <row r="5">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.671532846715329</v>
+        <v>0.995652173913043</v>
       </c>
     </row>
     <row r="6">
@@ -834,7 +834,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.875409754022471</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.5.4: desonn→DDESONN rename in performance_relevance_metrics.R + mirror Train_metrics.rds filtering for Test_metrics.rds (consistent metric/select filters & NA-safe pipeline)
</commit_message>
<xml_diff>
--- a/Rdata_predictions.xlsx
+++ b/Rdata_predictions.xlsx
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>230</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3">
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>519</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.99866667</v>
+        <v>0.73333333</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.54111406</v>
       </c>
     </row>
     <row r="8">
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.995671</v>
+        <v>0.88311688</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.9978308</v>
+        <v>0.67105263</v>
       </c>
     </row>
     <row r="10">
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.997333333333333</v>
+        <v>0.833333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -785,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.77319587628866</v>
       </c>
     </row>
     <row r="4">
@@ -793,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.991341991341991</v>
+        <v>0.649350649350649</v>
       </c>
     </row>
     <row r="5">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.995652173913043</v>
+        <v>0.705882352941177</v>
       </c>
     </row>
     <row r="6">
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +834,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0.880130787645239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>